<commit_message>
feat: finish the doc; wip: building the app don't work, have to fix: react router dom in electron app
</commit_message>
<xml_diff>
--- a/documentation/Planning_TPI_intro-Luca_Maggioli.xlsx
+++ b/documentation/Planning_TPI_intro-Luca_Maggioli.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nagragrp-my.sharepoint.com/personal/luca_maggioli_nagra_com/Documents/Desktop/TPI_intro/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maggioli\MyDesktop\Work\TPI_intro\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="175" documentId="8_{39ED9282-3F3A-42F2-9CB9-39D53CBFA76F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{033995B5-AE90-4457-AE1A-AA663BFCA364}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FC946E-6AB1-49D6-BDEF-1B31F2246F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{F6868423-5B24-42CE-9158-947897399ED9}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
   <si>
     <t>Taches à effectuer</t>
   </si>
@@ -76,9 +76,6 @@
     <t>15.09.2022</t>
   </si>
   <si>
-    <t>20.09.2022</t>
-  </si>
-  <si>
     <t>Création et réalisation du rapport</t>
   </si>
   <si>
@@ -128,6 +125,15 @@
   </si>
   <si>
     <t>Phase d'analyse des technologies à utiliser</t>
+  </si>
+  <si>
+    <t>21.09.20222</t>
+  </si>
+  <si>
+    <t>20.09.2023</t>
+  </si>
+  <si>
+    <t>Malade</t>
   </si>
 </sst>
 </file>
@@ -163,7 +169,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -173,6 +179,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFA8686"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -189,17 +201,53 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFA8686"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -223,6 +271,12 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFA8686"/>
+      <color rgb="FFFF6600"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -235,10 +289,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CF9ADE20-8AA5-4FFB-BAC8-55A81BBE75FA}" name="Table2" displayName="Table2" ref="A1:M19" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:M19" xr:uid="{CF9ADE20-8AA5-4FFB-BAC8-55A81BBE75FA}"/>
-  <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{CA3EBE62-94A4-4180-8666-4C2556054451}" name="Taches à effectuer" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CF9ADE20-8AA5-4FFB-BAC8-55A81BBE75FA}" name="Table2" displayName="Table2" ref="A1:N19" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:N19" xr:uid="{CF9ADE20-8AA5-4FFB-BAC8-55A81BBE75FA}"/>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{CA3EBE62-94A4-4180-8666-4C2556054451}" name="Taches à effectuer" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{E96C89DC-0A7C-4A1E-B341-50FEF3AC589B}" name="30.08.2022"/>
     <tableColumn id="3" xr3:uid="{D3B6EA26-F912-4FD2-B60F-D8CD78B3821A}" name="31.09.2022"/>
     <tableColumn id="4" xr3:uid="{3C51D906-4D3C-44F4-AFD5-E541FF350FAB}" name="01.09.2022"/>
@@ -250,7 +304,8 @@
     <tableColumn id="10" xr3:uid="{41E69F2A-84F6-46F7-93E8-67FC9767C71F}" name="13.09.2022"/>
     <tableColumn id="11" xr3:uid="{D9F0E820-6727-42F5-A614-4C53BB8F275F}" name="14.09.2022"/>
     <tableColumn id="12" xr3:uid="{2F88C950-BA01-4F9E-89CE-2C4EFF68D094}" name="15.09.2022"/>
-    <tableColumn id="13" xr3:uid="{4217217B-FBE4-4F72-89D6-2B7B84C9018E}" name="20.09.2022"/>
+    <tableColumn id="13" xr3:uid="{4217217B-FBE4-4F72-89D6-2B7B84C9018E}" name="20.09.2023" dataDxfId="0"/>
+    <tableColumn id="14" xr3:uid="{E6D0ADE3-2565-4650-A051-0FA43BD2CE89}" name="21.09.20222" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -553,19 +608,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07CA3C5D-4C1F-4C60-BF94-C9399AC6FD5D}">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="41.36328125" customWidth="1"/>
     <col min="2" max="13" width="12.6328125" customWidth="1"/>
+    <col min="14" max="14" width="12.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -602,11 +658,14 @@
       <c r="L1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -621,11 +680,14 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="1"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -638,11 +700,14 @@
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" s="4"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -655,11 +720,14 @@
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N4" s="4"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="4"/>
       <c r="E5" s="3"/>
@@ -670,11 +738,14 @@
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N5" s="3"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -686,11 +757,14 @@
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" s="3"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -703,16 +777,19 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="2"/>
+      <c r="E8" s="4"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -720,23 +797,30 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9" s="4"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -745,67 +829,111 @@
       <c r="F10" s="4"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M10" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="M11" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="G12" s="2"/>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="M12" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="M13" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N14" s="6"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L15" s="4"/>
+      <c r="M15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N15" s="4"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L16" s="4"/>
+      <c r="M16" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N17" s="4"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I14" s="2"/>
-      <c r="J14" s="4"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K15" s="4"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L16" s="4"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="L17" s="4"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
+      <c r="M18" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N18" s="4"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="M18" s="4"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="C19" s="4"/>
       <c r="E19" s="4"/>
       <c r="G19" s="4"/>
       <c r="I19" s="4"/>
       <c r="K19" s="4"/>
-      <c r="M19" s="4"/>
+      <c r="M19" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N19" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>